<commit_message>
atencion: base estable (store unificado, chips ≥65, inicio sin ficha)
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\QF-PRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043535D6-5E33-4232-888E-DC479E66286F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ADFE9D-E8C4-45F1-B91E-E88094BBB80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="243">
   <si>
     <t>FORMA</t>
   </si>
@@ -762,6 +762,9 @@
   </si>
   <si>
     <t>DROGA Z</t>
+  </si>
+  <si>
+    <t>UI</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -857,6 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,8 +1202,8 @@
   <dimension ref="A1:AH65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4731,7 +4735,7 @@
         <v>179</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>195</v>
@@ -4811,7 +4815,7 @@
         <v>179</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>195</v>
@@ -4890,7 +4894,7 @@
       <c r="C46" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E46" s="9" t="s">

</xml_diff>